<commit_message>
Adiciona programa principal e funcionalidade de análise de um mês individualmente
</commit_message>
<xml_diff>
--- a/Projetos/Projeto4/loot_rares.xlsx
+++ b/Projetos/Projeto4/loot_rares.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="230">
   <si>
     <t>Data</t>
   </si>
@@ -711,6 +711,12 @@
   </si>
   <si>
     <t>DEZEMBRO/2024</t>
+  </si>
+  <si>
+    <t>JANEIRO2025</t>
+  </si>
+  <si>
+    <t>service bakra ramiro</t>
   </si>
 </sst>
 </file>
@@ -718,7 +724,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -941,7 +947,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,7 +1239,7 @@
   <dimension ref="A1:H413"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2563,9 @@
       <c r="E52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="4"/>
+      <c r="F52" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4">
         <v>12</v>
@@ -2580,7 +2588,9 @@
       <c r="E53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="4"/>
+      <c r="F53" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4">
         <v>12</v>
@@ -3179,7 +3189,9 @@
       <c r="E76" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F76" s="4"/>
+      <c r="F76" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4">
         <v>7</v>
@@ -11850,9 +11862,8 @@
       <c r="C413" s="4">
         <v>2025</v>
       </c>
-      <c r="D413" s="25" t="str">
-        <f>CONCATENATE(B413,C413)</f>
-        <v>JANEIRO2025</v>
+      <c r="D413" s="25" t="s">
+        <v>228</v>
       </c>
       <c r="E413" s="1" t="s">
         <v>52</v>

</xml_diff>